<commit_message>
Separated codes for data cleaning, plotting and regressions.
</commit_message>
<xml_diff>
--- a/src/original_data/child_var_info.xlsx
+++ b/src/original_data/child_var_info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/berfinbinzet/Desktop/EPP_Project/project/Final_Project/src/original_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F5AE9C-2377-D94F-956C-7061F9D6323B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8E87AB-1458-F043-AA5D-EE21B71C4C60}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="100" windowWidth="26740" windowHeight="14580" xr2:uid="{795EDAA3-464B-8941-A715-B7883916D018}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>R0000100</t>
   </si>
@@ -48,9 +48,6 @@
     <t>C1DOB~Y</t>
   </si>
   <si>
-    <t>XRND</t>
-  </si>
-  <si>
     <t>nlsy_name</t>
   </si>
   <si>
@@ -67,6 +64,9 @@
   </si>
   <si>
     <t>first_child</t>
+  </si>
+  <si>
+    <t>invariant</t>
   </si>
 </sst>
 </file>
@@ -439,7 +439,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -449,16 +449,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.2">
@@ -469,10 +469,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1979</v>
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.2">
@@ -483,10 +483,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>